<commit_message>
Raphael and Xavier (Download pth file from the google drive and add it into the same directory as __init__.py
Due to LFS Limit exceeded, please download the best_model.pth file in this
google drive link: https://drive.google.com/file/d/1_SBTI1VXtjaZq5yGbIz5cBDTwSmS1mXJ/view?usp=sharing
</commit_message>
<xml_diff>
--- a/consumption_data.xlsx
+++ b/consumption_data.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Pellet Consumption" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name=" Leftover Pellets Over The Past Seven Days" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,113 +428,135 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Time</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Number of Pellets</t>
+          <t>first feed number of pellets left</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>second feed number of pellets left</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total feed pellets fed</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10:44:33</t>
+          <t>20 May</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="C2" t="n">
+        <v>30</v>
+      </c>
+      <c r="D2" t="n">
+        <v>400</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>10:44:37</t>
+          <t>21 May</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>40</v>
+      </c>
+      <c r="D3" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>10:44:42</t>
+          <t>22 May</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="C4" t="n">
+        <v>30</v>
+      </c>
+      <c r="D4" t="n">
+        <v>250</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>10:44:47</t>
+          <t>23 May</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" t="n">
+        <v>400</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>10:44:58</t>
+          <t>24 May</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="C6" t="n">
+        <v>40</v>
+      </c>
+      <c r="D6" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>10:45:01</t>
+          <t>25 May</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="C7" t="n">
+        <v>35</v>
+      </c>
+      <c r="D7" t="n">
+        <v>275</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>10:45:04</t>
+          <t>26 May</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>10:45:07</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>10:45:10</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10:45:13</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>